<commit_message>
work in progress to sync clocks
</commit_message>
<xml_diff>
--- a/UniformityIllusionPsychoPy/picPaths.xlsx
+++ b/UniformityIllusionPsychoPy/picPaths.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hesselmann\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hesselmann\Desktop\PsychoPyUniformityIllusion\UniformityIllusionPsychoPy\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,36 +24,156 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
-  <si>
-    <t>ImageFile</t>
-  </si>
-  <si>
-    <t>OldNew</t>
-  </si>
-  <si>
-    <t>old</t>
-  </si>
-  <si>
-    <t>new</t>
-  </si>
-  <si>
-    <t>C:\Users\hesselmann\Desktop\stimuli\1a.png</t>
-  </si>
-  <si>
-    <t>C:\Users\hesselmann\Desktop\stimuli\1b.png</t>
-  </si>
-  <si>
-    <t>C:\Users\hesselmann\Desktop\stimuli\2a.png</t>
-  </si>
-  <si>
-    <t>C:\Users\hesselmann\Desktop\stimuli\2b.png</t>
-  </si>
-  <si>
-    <t>C:\Users\hesselmann\Desktop\stimuli\3a.png</t>
-  </si>
-  <si>
-    <t>C:\Users\hesselmann\Desktop\stimuli\3b.png</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="50">
+  <si>
+    <t>AB</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>startImage</t>
+  </si>
+  <si>
+    <t>endImage</t>
+  </si>
+  <si>
+    <t>C:\Users\hesselmann\Desktop\PsychoPyUniformityIllusion\UniformityIllusionPsychoPy\Pics\1start.png</t>
+  </si>
+  <si>
+    <t>C:\Users\hesselmann\Desktop\PsychoPyUniformityIllusion\UniformityIllusionPsychoPy\Pics\1a.png</t>
+  </si>
+  <si>
+    <t>C:\Users\hesselmann\Desktop\PsychoPyUniformityIllusion\UniformityIllusionPsychoPy\Pics\1b.png</t>
+  </si>
+  <si>
+    <t>C:\Users\hesselmann\Desktop\PsychoPyUniformityIllusion\UniformityIllusionPsychoPy\Pics\2start.png</t>
+  </si>
+  <si>
+    <t>C:\Users\hesselmann\Desktop\PsychoPyUniformityIllusion\UniformityIllusionPsychoPy\Pics\2a.png</t>
+  </si>
+  <si>
+    <t>C:\Users\hesselmann\Desktop\PsychoPyUniformityIllusion\UniformityIllusionPsychoPy\Pics\2b.png</t>
+  </si>
+  <si>
+    <t>C:\Users\hesselmann\Desktop\PsychoPyUniformityIllusion\UniformityIllusionPsychoPy\Pics\3start.png</t>
+  </si>
+  <si>
+    <t>C:\Users\hesselmann\Desktop\PsychoPyUniformityIllusion\UniformityIllusionPsychoPy\Pics\3a.png</t>
+  </si>
+  <si>
+    <t>C:\Users\hesselmann\Desktop\PsychoPyUniformityIllusion\UniformityIllusionPsychoPy\Pics\3b.png</t>
+  </si>
+  <si>
+    <t>C:\Users\hesselmann\Desktop\PsychoPyUniformityIllusion\UniformityIllusionPsychoPy\Pics\4a.png</t>
+  </si>
+  <si>
+    <t>C:\Users\hesselmann\Desktop\PsychoPyUniformityIllusion\UniformityIllusionPsychoPy\Pics\4b.png</t>
+  </si>
+  <si>
+    <t>C:\Users\hesselmann\Desktop\PsychoPyUniformityIllusion\UniformityIllusionPsychoPy\Pics\5a.png</t>
+  </si>
+  <si>
+    <t>C:\Users\hesselmann\Desktop\PsychoPyUniformityIllusion\UniformityIllusionPsychoPy\Pics\5b.png</t>
+  </si>
+  <si>
+    <t>C:\Users\hesselmann\Desktop\PsychoPyUniformityIllusion\UniformityIllusionPsychoPy\Pics\6a.png</t>
+  </si>
+  <si>
+    <t>C:\Users\hesselmann\Desktop\PsychoPyUniformityIllusion\UniformityIllusionPsychoPy\Pics\6b.png</t>
+  </si>
+  <si>
+    <t>C:\Users\hesselmann\Desktop\PsychoPyUniformityIllusion\UniformityIllusionPsychoPy\Pics\4start.png</t>
+  </si>
+  <si>
+    <t>C:\Users\hesselmann\Desktop\PsychoPyUniformityIllusion\UniformityIllusionPsychoPy\Pics\5start.png</t>
+  </si>
+  <si>
+    <t>C:\Users\hesselmann\Desktop\PsychoPyUniformityIllusion\UniformityIllusionPsychoPy\Pics\6start.png</t>
+  </si>
+  <si>
+    <t>C:\Users\hesselmann\Desktop\PsychoPyUniformityIllusion\UniformityIllusionPsychoPy\Pics\7start.png</t>
+  </si>
+  <si>
+    <t>C:\Users\hesselmann\Desktop\PsychoPyUniformityIllusion\UniformityIllusionPsychoPy\Pics\7a.png</t>
+  </si>
+  <si>
+    <t>C:\Users\hesselmann\Desktop\PsychoPyUniformityIllusion\UniformityIllusionPsychoPy\Pics\7b.png</t>
+  </si>
+  <si>
+    <t>C:\Users\hesselmann\Desktop\PsychoPyUniformityIllusion\UniformityIllusionPsychoPy\Pics\8start.png</t>
+  </si>
+  <si>
+    <t>C:\Users\hesselmann\Desktop\PsychoPyUniformityIllusion\UniformityIllusionPsychoPy\Pics\8a.png</t>
+  </si>
+  <si>
+    <t>C:\Users\hesselmann\Desktop\PsychoPyUniformityIllusion\UniformityIllusionPsychoPy\Pics\8b.png</t>
+  </si>
+  <si>
+    <t>C:\Users\hesselmann\Desktop\PsychoPyUniformityIllusion\UniformityIllusionPsychoPy\Pics\9start.png</t>
+  </si>
+  <si>
+    <t>C:\Users\hesselmann\Desktop\PsychoPyUniformityIllusion\UniformityIllusionPsychoPy\Pics\9a.png</t>
+  </si>
+  <si>
+    <t>C:\Users\hesselmann\Desktop\PsychoPyUniformityIllusion\UniformityIllusionPsychoPy\Pics\9b.png</t>
+  </si>
+  <si>
+    <t>C:\Users\hesselmann\Desktop\PsychoPyUniformityIllusion\UniformityIllusionPsychoPy\Pics\10start.png</t>
+  </si>
+  <si>
+    <t>C:\Users\hesselmann\Desktop\PsychoPyUniformityIllusion\UniformityIllusionPsychoPy\Pics\10a.png</t>
+  </si>
+  <si>
+    <t>C:\Users\hesselmann\Desktop\PsychoPyUniformityIllusion\UniformityIllusionPsychoPy\Pics\10b.png</t>
+  </si>
+  <si>
+    <t>C:\Users\hesselmann\Desktop\PsychoPyUniformityIllusion\UniformityIllusionPsychoPy\Pics\11start.png</t>
+  </si>
+  <si>
+    <t>C:\Users\hesselmann\Desktop\PsychoPyUniformityIllusion\UniformityIllusionPsychoPy\Pics\11a.png</t>
+  </si>
+  <si>
+    <t>C:\Users\hesselmann\Desktop\PsychoPyUniformityIllusion\UniformityIllusionPsychoPy\Pics\11b.png</t>
+  </si>
+  <si>
+    <t>C:\Users\hesselmann\Desktop\PsychoPyUniformityIllusion\UniformityIllusionPsychoPy\Pics\12start.png</t>
+  </si>
+  <si>
+    <t>C:\Users\hesselmann\Desktop\PsychoPyUniformityIllusion\UniformityIllusionPsychoPy\Pics\12a.png</t>
+  </si>
+  <si>
+    <t>C:\Users\hesselmann\Desktop\PsychoPyUniformityIllusion\UniformityIllusionPsychoPy\Pics\12b.png</t>
+  </si>
+  <si>
+    <t>C:\Users\hesselmann\Desktop\PsychoPyUniformityIllusion\UniformityIllusionPsychoPy\Pics\13start.png</t>
+  </si>
+  <si>
+    <t>C:\Users\hesselmann\Desktop\PsychoPyUniformityIllusion\UniformityIllusionPsychoPy\Pics\13a.png</t>
+  </si>
+  <si>
+    <t>C:\Users\hesselmann\Desktop\PsychoPyUniformityIllusion\UniformityIllusionPsychoPy\Pics\13b.png</t>
+  </si>
+  <si>
+    <t>C:\Users\hesselmann\Desktop\PsychoPyUniformityIllusion\UniformityIllusionPsychoPy\Pics\14start.png</t>
+  </si>
+  <si>
+    <t>C:\Users\hesselmann\Desktop\PsychoPyUniformityIllusion\UniformityIllusionPsychoPy\Pics\14a.png</t>
+  </si>
+  <si>
+    <t>C:\Users\hesselmann\Desktop\PsychoPyUniformityIllusion\UniformityIllusionPsychoPy\Pics\14b.png</t>
+  </si>
+  <si>
+    <t>C:\Users\hesselmann\Desktop\PsychoPyUniformityIllusion\UniformityIllusionPsychoPy\Pics\15start.png</t>
+  </si>
+  <si>
+    <t>C:\Users\hesselmann\Desktop\PsychoPyUniformityIllusion\UniformityIllusionPsychoPy\Pics\15a.png</t>
+  </si>
+  <si>
+    <t>C:\Users\hesselmann\Desktop\PsychoPyUniformityIllusion\UniformityIllusionPsychoPy\Pics\15b.png</t>
   </si>
 </sst>
 </file>
@@ -372,71 +492,303 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="42.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="97.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="94.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>3</v>
+        <v>13</v>
+      </c>
+      <c r="C7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>29</v>
+      </c>
+      <c r="B19" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>35</v>
+      </c>
+      <c r="B22" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>35</v>
+      </c>
+      <c r="B23" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>38</v>
+      </c>
+      <c r="B24" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>38</v>
+      </c>
+      <c r="B25" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>41</v>
+      </c>
+      <c r="B26" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>41</v>
+      </c>
+      <c r="B27" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>44</v>
+      </c>
+      <c r="B28" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>44</v>
+      </c>
+      <c r="B29" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>47</v>
+      </c>
+      <c r="B30" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>47</v>
+      </c>
+      <c r="B31" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add discrete opacity steps
</commit_message>
<xml_diff>
--- a/UniformityIllusionPsychoPy/picPaths.xlsx
+++ b/UniformityIllusionPsychoPy/picPaths.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="52">
   <si>
     <t>AB</t>
   </si>
@@ -174,6 +174,12 @@
   </si>
   <si>
     <t>C:\Users\hesselmann\Desktop\PsychoPyUniformityIllusion\UniformityIllusionPsychoPy\Pics\15b.png</t>
+  </si>
+  <si>
+    <t>midImage</t>
+  </si>
+  <si>
+    <t>C:\Users\hesselmann\Desktop\PsychoPyUniformityIllusion\UniformityIllusionPsychoPy\Pics\12bapng</t>
   </si>
 </sst>
 </file>
@@ -492,30 +498,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C31"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="97.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="94.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="93" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="93" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
       <c r="B1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -523,21 +533,27 @@
         <v>6</v>
       </c>
       <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -545,21 +561,27 @@
         <v>9</v>
       </c>
       <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
       <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
         <v>10</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -567,21 +589,27 @@
         <v>12</v>
       </c>
       <c r="C6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
       <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" t="s">
         <v>13</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -589,21 +617,27 @@
         <v>14</v>
       </c>
       <c r="C8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>20</v>
       </c>
       <c r="B9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" t="s">
         <v>15</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -611,21 +645,27 @@
         <v>16</v>
       </c>
       <c r="C10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>21</v>
       </c>
       <c r="B11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" t="s">
         <v>17</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -633,161 +673,221 @@
         <v>18</v>
       </c>
       <c r="C12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>22</v>
       </c>
       <c r="B13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" t="s">
         <v>19</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>23</v>
       </c>
       <c r="B14" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>23</v>
       </c>
       <c r="B15" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>26</v>
       </c>
       <c r="B16" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>26</v>
       </c>
       <c r="B17" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>29</v>
       </c>
       <c r="B18" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>29</v>
       </c>
       <c r="B19" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>32</v>
       </c>
       <c r="B20" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>32</v>
       </c>
       <c r="B21" t="s">
+        <v>33</v>
+      </c>
+      <c r="C21" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>35</v>
       </c>
       <c r="B22" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>35</v>
       </c>
       <c r="B23" t="s">
+        <v>36</v>
+      </c>
+      <c r="C23" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>38</v>
       </c>
       <c r="B24" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>38</v>
       </c>
       <c r="B25" t="s">
+        <v>51</v>
+      </c>
+      <c r="C25" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>41</v>
       </c>
       <c r="B26" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>41</v>
       </c>
       <c r="B27" t="s">
+        <v>42</v>
+      </c>
+      <c r="C27" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>44</v>
       </c>
       <c r="B28" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>44</v>
       </c>
       <c r="B29" t="s">
+        <v>45</v>
+      </c>
+      <c r="C29" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>47</v>
       </c>
       <c r="B30" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C30" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>47</v>
       </c>
       <c r="B31" t="s">
+        <v>48</v>
+      </c>
+      <c r="C31" t="s">
         <v>49</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add annotations for keypress
</commit_message>
<xml_diff>
--- a/UniformityIllusionPsychoPy/picPaths.xlsx
+++ b/UniformityIllusionPsychoPy/picPaths.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="51">
   <si>
     <t>AB</t>
   </si>
@@ -177,9 +177,6 @@
   </si>
   <si>
     <t>midImage</t>
-  </si>
-  <si>
-    <t>C:\Users\hesselmann\Desktop\PsychoPyUniformityIllusion\UniformityIllusionPsychoPy\Pics\12bapng</t>
   </si>
 </sst>
 </file>
@@ -500,8 +497,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -819,7 +816,7 @@
         <v>38</v>
       </c>
       <c r="B25" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="C25" t="s">
         <v>40</v>

</xml_diff>